<commit_message>
Se agrega validaciones de API
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/apiData.xlsx
+++ b/src/test/resources/datadriven/apiData.xlsx
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
-  <si>
-    <t>nombrePeticion</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>Headers</t>
   </si>
@@ -47,15 +44,6 @@
     <t>Body</t>
   </si>
   <si>
-    <t>fileURL</t>
-  </si>
-  <si>
-    <t>pathParams</t>
-  </si>
-  <si>
-    <t>respuestasEsperadas</t>
-  </si>
-  <si>
     <t>Get a Single Member</t>
   </si>
   <si>
@@ -80,27 +68,6 @@
     <t>Download a File</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>http://localhost:5002/api/members/1</t>
-  </si>
-  <si>
-    <t>http://localhost:5002/api/authors/1</t>
-  </si>
-  <si>
-    <t>http://localhost:5002/api/members/40</t>
-  </si>
-  <si>
-    <t>http://localhost:5002/api/members</t>
-  </si>
-  <si>
-    <t>http://localhost:5002/api/upload</t>
-  </si>
-  <si>
-    <t>http://localhost:5002/api/download?name=Yey.jpg</t>
-  </si>
-  <si>
     <t>Metodo</t>
   </si>
   <si>
@@ -146,15 +113,6 @@
     <t>msg</t>
   </si>
   <si>
-    <t>Member with id 4 is deleted successfully</t>
-  </si>
-  <si>
-    <t>Member with id 5 is updated successfully</t>
-  </si>
-  <si>
-    <t>http://localhost:5002/api/members/5</t>
-  </si>
-  <si>
     <t>name#gender</t>
   </si>
   <si>
@@ -173,10 +131,82 @@
     <t>Tiendas Éxito</t>
   </si>
   <si>
-    <t>usuario</t>
-  </si>
-  <si>
-    <t>miguel</t>
+    <t>/api/members/1</t>
+  </si>
+  <si>
+    <t>/api/authors/1</t>
+  </si>
+  <si>
+    <t>/api/members</t>
+  </si>
+  <si>
+    <t>/api/upload</t>
+  </si>
+  <si>
+    <t>/api/download?name=Yey.jpg</t>
+  </si>
+  <si>
+    <t>EndPoint</t>
+  </si>
+  <si>
+    <t>FileURL</t>
+  </si>
+  <si>
+    <t>PathParams</t>
+  </si>
+  <si>
+    <t>RespuestasEsperadas</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>NombrePeticion</t>
+  </si>
+  <si>
+    <t>/api/members/20</t>
+  </si>
+  <si>
+    <t>/api/members/21</t>
+  </si>
+  <si>
+    <t>Member with id 20 is updated successfully</t>
+  </si>
+  <si>
+    <t>Member with id 21 is updated successfully</t>
+  </si>
+  <si>
+    <t>miguel1</t>
+  </si>
+  <si>
+    <t>miguel2</t>
+  </si>
+  <si>
+    <t>miguel3</t>
+  </si>
+  <si>
+    <t>miguel4</t>
+  </si>
+  <si>
+    <t>miguel5</t>
+  </si>
+  <si>
+    <t>miguel6</t>
+  </si>
+  <si>
+    <t>miguel7</t>
+  </si>
+  <si>
+    <t>miguel8</t>
+  </si>
+  <si>
+    <t>/api/members/5</t>
+  </si>
+  <si>
+    <t>Member with id 5 is deleted successfully</t>
+  </si>
+  <si>
+    <t>C:/Users/Usuario/Documents/Automation_Web/src/test/resources/jpg/demo.jpg</t>
   </si>
 </sst>
 </file>
@@ -742,15 +772,15 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:I9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <tableColumns count="9">
-    <tableColumn id="1" name="nombrePeticion" dataDxfId="8"/>
+    <tableColumn id="1" name="NombrePeticion" dataDxfId="8"/>
     <tableColumn id="8" name="Metodo" dataDxfId="7"/>
-    <tableColumn id="7" name="URL" dataDxfId="6"/>
+    <tableColumn id="7" name="EndPoint" dataDxfId="6"/>
     <tableColumn id="2" name="Headers" dataDxfId="5"/>
     <tableColumn id="3" name="Body" dataDxfId="4"/>
-    <tableColumn id="4" name="fileURL" dataDxfId="3"/>
-    <tableColumn id="5" name="pathParams" dataDxfId="2"/>
-    <tableColumn id="6" name="respuestasEsperadas" dataDxfId="1"/>
-    <tableColumn id="9" name="usuario" dataDxfId="0"/>
+    <tableColumn id="4" name="FileURL" dataDxfId="3"/>
+    <tableColumn id="5" name="PathParams" dataDxfId="2"/>
+    <tableColumn id="6" name="RespuestasEsperadas" dataDxfId="1"/>
+    <tableColumn id="9" name="Usuario" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1055,7 +1085,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1064,60 +1096,60 @@
     <col min="3" max="3" width="42.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>46</v>
@@ -1125,191 +1157,193 @@
     </row>
     <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>24</v>
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="I5" s="11" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>29</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
       <c r="I6" s="11" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>30</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="C9" s="8" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
+      <c r="G9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="I9" s="11" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="C2" r:id="rId1" display="http://localhost:5002/api/members/1"/>
+    <hyperlink ref="C3" r:id="rId2" display="http://localhost:5002/api/authors/1"/>
+    <hyperlink ref="C7" r:id="rId3" display="http://localhost:5002/api/members/40"/>
+    <hyperlink ref="C9" r:id="rId4" display="http://localhost:5002/api/members/5"/>
+    <hyperlink ref="C8" r:id="rId5" display="http://localhost:5002/api/members/5"/>
+    <hyperlink ref="C4" r:id="rId6" display="http://localhost:5002/api/members"/>
+    <hyperlink ref="C5" r:id="rId7" display="http://localhost:5002/api/upload"/>
+    <hyperlink ref="C6" r:id="rId8" display="http://localhost:5002/api/download?name=Yey.jpg"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1331,12 +1365,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ultimo commit - prueba tecnica
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/apiData.xlsx
+++ b/src/test/resources/datadriven/apiData.xlsx
@@ -200,13 +200,13 @@
     <t>miguel8</t>
   </si>
   <si>
-    <t>/api/members/5</t>
-  </si>
-  <si>
-    <t>Member with id 5 is deleted successfully</t>
-  </si>
-  <si>
     <t>C:/Users/Usuario/Documents/Automation_Web/src/test/resources/jpg/demo.jpg</t>
+  </si>
+  <si>
+    <t>/api/members/40</t>
+  </si>
+  <si>
+    <t>Member with id 40 is deleted successfully</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1086,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>28</v>
@@ -1263,7 +1263,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>16</v>
@@ -1274,7 +1274,7 @@
         <v>24</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>49</v>

</xml_diff>